<commit_message>
Quote revision system now increments the revision number on each save.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>Section</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Dates should not be able to be put into invalid states (eg expiration date can be before the creation date)</t>
+  </si>
+  <si>
+    <t>Complete</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -474,7 +477,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Pressing enter in boxes that format as currency now formats the dollar amount nicely.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Title</t>
   </si>
@@ -103,6 +103,39 @@
   </si>
   <si>
     <t>Completed - Mar 8, 2010 (still need to go through and remove hard codes throughout program)</t>
+  </si>
+  <si>
+    <t>Move 'view' buttons</t>
+  </si>
+  <si>
+    <t>For stuff like quotes and invoices, it would be nice to have the "View printout"  button in the yellow-ish bar that includes the save button so that it can be pressed without going back to the first tab all the time.</t>
+  </si>
+  <si>
+    <t>Most users I have observered will instinctively hit enter after they have enter a value into any of the fields that acces a dollar amount, likely expecting it to format it correctly. Currently nothing happens when they do this, so it would be nice if it did.</t>
+  </si>
+  <si>
+    <t>Accept metric or english measurements</t>
+  </si>
+  <si>
+    <t>The system should be able to accept both metric and imperial measurements as both are used. The system should ideally store in metric and convert to imperial upon request.</t>
+  </si>
+  <si>
+    <t>Quote condition selection</t>
+  </si>
+  <si>
+    <t>When one of the quote condition text boxes recieves focus, it should automatically check the checkbox associated with it if it isn't already, as it is expected that if the user is editing the text they intent to include the condition and might forget to check it manually.</t>
+  </si>
+  <si>
+    <t>Press enter in currency fields</t>
+  </si>
+  <si>
+    <t>Completed - Mar 10, 2010</t>
+  </si>
+  <si>
+    <t>Differentiate read-only textboxes</t>
+  </si>
+  <si>
+    <t>Some entry forms have read-only fields, but it isn't obvious that you can't edit them until you try. It would be nice to change the style of these boxes so that the user knows they aren't editable.</t>
   </si>
 </sst>
 </file>
@@ -469,15 +502,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="38.28515625" style="5" customWidth="1"/>
     <col min="2" max="2" width="87.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="31.5703125" style="5" customWidth="1"/>
   </cols>
@@ -600,6 +633,61 @@
         <v>23</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Editing a quote condition's text now automatically includes that condition in the quote.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -505,7 +505,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,7 +677,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>11</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All read-only text fields should now include the ReadOnly style.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Title</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>When saving to PDF in the DocumentViewer window a default filename should be used. For example when printing quotes, the default Filename should be Quote #[num]-[rev].pdf.</t>
-  </si>
-  <si>
-    <t>Partial - Done for quote printouts</t>
   </si>
   <si>
     <t>Highlight all in text fields</t>
@@ -505,7 +502,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,18 +525,18 @@
     </row>
     <row r="2" spans="1:3" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="6" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -556,139 +553,139 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="C6" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C7" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C14" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>35</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C16" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bug fixes in the import system.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
   <si>
     <t>Title</t>
   </si>
@@ -143,50 +142,34 @@
   </si>
   <si>
     <t>There should be a button or checkbox in the quotes section that changes the quote price text field and calculates the price based on the commodity movement and supplement costs.</t>
+  </si>
+  <si>
+    <t>Complete - Mar 15, 2010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00" numFmtId="165"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="SimSun"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -198,7 +181,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -206,84 +189,347 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1F497D" mc:Ignorable=""/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="EEECE1" mc:Ignorable=""/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4F81BD" mc:Ignorable=""/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0504D" mc:Ignorable=""/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="9BBB59" mc:Ignorable=""/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="8064A2" mc:Ignorable=""/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4BACC6" mc:Ignorable=""/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="F79646" mc:Ignorable=""/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable=""/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="800080" mc:Ignorable=""/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.0235294117647"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="89.4039215686275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.1803921568627"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.44705882352941"/>
+    <col min="1" max="1" width="39" style="1"/>
+    <col min="2" max="2" width="89.375" style="2"/>
+    <col min="3" max="3" width="32.125" style="1"/>
+    <col min="4" max="1025" width="9.5"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="5">
+    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -294,7 +540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="2" s="8">
+    <row r="2" spans="1:3" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
@@ -305,7 +551,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="3">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -316,7 +562,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="4">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -327,7 +573,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="68.65" outlineLevel="0" r="5">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -338,7 +584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -346,10 +592,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="7">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -360,7 +606,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="8">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
@@ -371,7 +617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="9">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>22</v>
       </c>
@@ -382,7 +628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="10">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
@@ -393,7 +639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="11">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>27</v>
       </c>
@@ -404,7 +650,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="12">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -415,7 +661,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="13">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
@@ -426,7 +672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="14">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
@@ -437,7 +683,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="15">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>35</v>
       </c>
@@ -448,7 +694,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="16">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>37</v>
       </c>
@@ -459,7 +705,7 @@
         <v>39</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="17">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>40</v>
       </c>
@@ -471,62 +717,39 @@
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.44705882352941"/>
+    <col min="1" max="1025" width="9.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.44705882352941"/>
+    <col min="1" max="1025" width="9.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Quote's now have an itemized billing option.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Title</t>
   </si>
@@ -145,6 +145,9 @@
   </si>
   <si>
     <t>Complete - Mar 15, 2010</t>
+  </si>
+  <si>
+    <t>WONTFIX</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +617,7 @@
         <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated an important default configuration setting.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>Title</t>
   </si>
@@ -151,6 +151,12 @@
   </si>
   <si>
     <t>Completed - Mar 16, 2010</t>
+  </si>
+  <si>
+    <t>Progress bar or output for PDF creator</t>
+  </si>
+  <si>
+    <t>When clicking the "Create PDF" button in the document viewer, the user is not given any indication of what is happening. It would be nice if there were a progress bar or output window showing what is happening.</t>
   </si>
 </sst>
 </file>
@@ -521,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,6 +726,17 @@
       </c>
       <c r="C17" s="1" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Loads page now allows commodities to be added or removed from loads.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
   <si>
     <t>Title</t>
   </si>
@@ -173,50 +172,34 @@
   </si>
   <si>
     <t>When creating loads in the job section, it would be nice if the list of commodities was shown so that they can quickly be added.</t>
+  </si>
+  <si>
+    <t>Completed - Mar 29, 2010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="0.00" numFmtId="165"/>
-  </numFmts>
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="SimSun"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="true"/>
-      <color rgb="00000000"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -228,7 +211,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalDown="false" diagonalUp="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -236,78 +219,341 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="true" borderId="0" fillId="0" fontId="0" numFmtId="164">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="43"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="41"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="44"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="165" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="true"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
-    <cellStyle builtinId="3" customBuiltin="false" name="Comma" xfId="15"/>
-    <cellStyle builtinId="6" customBuiltin="false" name="Comma [0]" xfId="16"/>
-    <cellStyle builtinId="4" customBuiltin="false" name="Currency" xfId="17"/>
-    <cellStyle builtinId="7" customBuiltin="false" name="Currency [0]" xfId="18"/>
-    <cellStyle builtinId="5" customBuiltin="false" name="Percent" xfId="19"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="1F497D" mc:Ignorable=""/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="EEECE1" mc:Ignorable=""/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4F81BD" mc:Ignorable=""/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="C0504D" mc:Ignorable=""/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="9BBB59" mc:Ignorable=""/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="8064A2" mc:Ignorable=""/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="4BACC6" mc:Ignorable=""/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="F79646" mc:Ignorable=""/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0000FF" mc:Ignorable=""/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="800080" mc:Ignorable=""/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="000000" mc:Ignorable="">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="39.1450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="89.7137254901961"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="32.243137254902"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="9.53725490196078"/>
+    <col min="1" max="1" width="39.125" style="1"/>
+    <col min="2" max="2" width="89.75" style="2"/>
+    <col min="3" max="3" width="32.25" style="1"/>
+    <col min="4" max="1025" width="9.5"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="1" s="5">
+    <row r="1" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -318,7 +564,7 @@
         <v>2</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="2" s="6">
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -329,7 +575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="3">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -340,7 +586,7 @@
         <v>8</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="4">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -351,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="55.2" outlineLevel="0" r="5">
+    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -362,7 +608,7 @@
         <v>14</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -373,7 +619,7 @@
         <v>17</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -384,7 +630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="8">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -395,7 +641,7 @@
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="9">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
@@ -406,7 +652,7 @@
         <v>26</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="10">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -417,7 +663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="11">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
@@ -428,7 +674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="12">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>31</v>
       </c>
@@ -439,7 +685,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="13">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
@@ -450,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="14">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
@@ -461,7 +707,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="15">
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
@@ -472,7 +718,7 @@
         <v>11</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="16">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -483,7 +729,7 @@
         <v>41</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="17">
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
@@ -494,7 +740,7 @@
         <v>44</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="41.75" outlineLevel="0" r="18">
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -505,7 +751,7 @@
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="19">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -516,7 +762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="28.35" outlineLevel="0" r="20">
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>50</v>
       </c>
@@ -524,66 +770,43 @@
         <v>51</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.53725490196078"/>
+    <col min="1" max="1025" width="9.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.53725490196078"/>
+    <col min="1" max="1025" width="9.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="0" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="1" scale="100" useFirstPageNumber="false" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Some areas now display text that says "Saved" when the form data is saved (not sure if this will be the final solution). Also fixed an unreported bug that was discovered.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9114"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Title</t>
   </si>
@@ -196,6 +196,12 @@
   </si>
   <si>
     <t>Completed - March 29, 2010</t>
+  </si>
+  <si>
+    <t>Standardize on confirmation dialogs</t>
+  </si>
+  <si>
+    <t>There are many places in the system where there are "remove" or "delete" buttons. Some of these buttons will open a dialog box asking the user to confirm the action, but others do not. It should be the same behaviour everywhere.</t>
   </si>
 </sst>
 </file>
@@ -560,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -824,6 +830,17 @@
         <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.15">
+      <c r="A24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
When printing dispatches, the user is now asked if a "driver's copy" should be included.
</commit_message>
<xml_diff>
--- a/Documents/ToDo.xlsx
+++ b/Documents/ToDo.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
   <si>
     <t>Title</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>There are many places in the system where there are "remove" or "delete" buttons. Some of these buttons will open a dialog box asking the user to confirm the action, but others do not. It should be the same behaviour everywhere.</t>
+  </si>
+  <si>
+    <t>Completed - March 30, 2010</t>
   </si>
 </sst>
 </file>
@@ -830,7 +833,7 @@
         <v>58</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>20</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.15">

</xml_diff>